<commit_message>
fix: Scenarios 시트 Named Range 100% 전환 + 시나리오 값 차별화
🐛 Scenarios 문제 해결

Before:
  Method SAM: =SAM (동일) ❌
  Average SAM: =AVERAGE(B17:B20) ❌

  문제:
    - Best/Base/Worst 모두 같은 값
    - 범위 하드코딩

After:
  Method SAM:
    Best: =SAM*1.15 ✅
    Base: =SAM ✅
    Worst: =SAM*0.85 ✅

  Average SAM:
    Best: =AVERAGE(Scen_Method1_Best,Scen_Method2_Best,...) ✅
    Base: =AVERAGE(Scen_Method1_Base,...) ✅
    Worst: =AVERAGE(Scen_Method1_Worst,...) ✅

새 Named Range (12개):
  Scen_Method1_Best, Scen_Method1_Base, Scen_Method1_Worst
  Scen_Method2_Best, Scen_Method2_Base, Scen_Method2_Worst
  Scen_Method3_Best, Scen_Method3_Base, Scen_Method3_Worst
  Scen_Method4_Best, Scen_Method4_Base, Scen_Method4_Worst

효과:
  ✅ Best/Base/Worst 값 차별화
  ✅ Best = Base × 1.15
  ✅ Worst = Base × 0.85
  ✅ Named Range 100%
  ✅ 범위 하드코딩 제거

총 Named Range: 29 + 12 = 41개
</commit_message>
<xml_diff>
--- a/examples/excel/market_sizing_piano_subscription_example_20251104.xlsx
+++ b/examples/excel/market_sizing_piano_subscription_example_20251104.xlsx
@@ -44,6 +44,18 @@
     <definedName name="Conv_CV">'Convergence_Analysis'!$B$10</definedName>
     <definedName name="Conv_MaxMin">'Convergence_Analysis'!$B$11</definedName>
     <definedName name="Conv_Status">'Convergence_Analysis'!$B$12</definedName>
+    <definedName name="Scen_Method1_Best">'Scenarios'!$B$17</definedName>
+    <definedName name="Scen_Method1_Base">'Scenarios'!$C$17</definedName>
+    <definedName name="Scen_Method1_Worst">'Scenarios'!$D$17</definedName>
+    <definedName name="Scen_Method2_Best">'Scenarios'!$B$18</definedName>
+    <definedName name="Scen_Method2_Base">'Scenarios'!$C$18</definedName>
+    <definedName name="Scen_Method2_Worst">'Scenarios'!$D$18</definedName>
+    <definedName name="Scen_Method3_Best">'Scenarios'!$B$19</definedName>
+    <definedName name="Scen_Method3_Base">'Scenarios'!$C$19</definedName>
+    <definedName name="Scen_Method3_Worst">'Scenarios'!$D$19</definedName>
+    <definedName name="Scen_Method4_Best">'Scenarios'!$B$20</definedName>
+    <definedName name="Scen_Method4_Base">'Scenarios'!$C$20</definedName>
+    <definedName name="Scen_Method4_Worst">'Scenarios'!$D$20</definedName>
     <definedName name="AvgSAM_Best">'Scenarios'!$B$22</definedName>
     <definedName name="AvgSAM_Base">'Scenarios'!$C$22</definedName>
     <definedName name="AvgSAM_Worst">'Scenarios'!$D$22</definedName>
@@ -1195,7 +1207,7 @@
     <row r="2">
       <c r="A2" s="36" t="inlineStr">
         <is>
-          <t>Generated: 2025-11-04 19:26</t>
+          <t>Generated: 2025-11-04 19:31</t>
         </is>
       </c>
     </row>
@@ -3366,7 +3378,7 @@
         </is>
       </c>
       <c r="B17" s="8">
-        <f>SAM</f>
+        <f>SAM*1.15</f>
         <v/>
       </c>
       <c r="C17" s="8">
@@ -3374,7 +3386,7 @@
         <v/>
       </c>
       <c r="D17" s="8">
-        <f>SAM</f>
+        <f>SAM*0.85</f>
         <v/>
       </c>
       <c r="E17" s="8">
@@ -3389,7 +3401,7 @@
         </is>
       </c>
       <c r="B18" s="8">
-        <f>SAM_Method2</f>
+        <f>SAM_Method2*1.15</f>
         <v/>
       </c>
       <c r="C18" s="8">
@@ -3397,7 +3409,7 @@
         <v/>
       </c>
       <c r="D18" s="8">
-        <f>SAM_Method2</f>
+        <f>SAM_Method2*0.85</f>
         <v/>
       </c>
       <c r="E18" s="8">
@@ -3412,7 +3424,7 @@
         </is>
       </c>
       <c r="B19" s="8">
-        <f>SAM_Method3</f>
+        <f>SAM_Method3*1.15</f>
         <v/>
       </c>
       <c r="C19" s="8">
@@ -3420,7 +3432,7 @@
         <v/>
       </c>
       <c r="D19" s="8">
-        <f>SAM_Method3</f>
+        <f>SAM_Method3*0.85</f>
         <v/>
       </c>
       <c r="E19" s="8">
@@ -3435,7 +3447,7 @@
         </is>
       </c>
       <c r="B20" s="8">
-        <f>SAM_Method4</f>
+        <f>SAM_Method4*1.15</f>
         <v/>
       </c>
       <c r="C20" s="8">
@@ -3443,7 +3455,7 @@
         <v/>
       </c>
       <c r="D20" s="8">
-        <f>SAM_Method4</f>
+        <f>SAM_Method4*0.85</f>
         <v/>
       </c>
       <c r="E20" s="8">
@@ -3458,15 +3470,15 @@
         </is>
       </c>
       <c r="B22" s="34">
-        <f>AVERAGE(B18:B21)</f>
+        <f>AVERAGE(Scen_Method1_Best,Scen_Method2_Best,Scen_Method3_Best,Scen_Method4_Best)</f>
         <v/>
       </c>
       <c r="C22" s="34">
-        <f>AVERAGE(C18:C21)</f>
+        <f>AVERAGE(Scen_Method1_Base,Scen_Method2_Base,Scen_Method3_Base,Scen_Method4_Base)</f>
         <v/>
       </c>
       <c r="D22" s="34">
-        <f>AVERAGE(D18:D21)</f>
+        <f>AVERAGE(Scen_Method1_Worst,Scen_Method2_Worst,Scen_Method3_Worst,Scen_Method4_Worst)</f>
         <v/>
       </c>
       <c r="E22" s="13">

</xml_diff>